<commit_message>
Pipeline parameter population fix fixed
</commit_message>
<xml_diff>
--- a/PCF-exporter/PCF_DEVELOPEMENT_01.xlsx
+++ b/PCF-exporter/PCF_DEVELOPEMENT_01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pcf-exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\PCF-exporter\PCF-exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMP" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="TYPES" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="PCF_OVERVIEW" localSheetId="0">COMP!$A$1:$H$44</definedName>
+    <definedName name="PCF_OVERVIEW" localSheetId="0">COMP!$A$1:$I$44</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="181">
   <si>
     <t>ELBW</t>
   </si>
@@ -554,6 +554,63 @@
   </si>
   <si>
     <t>Piping System: Fjernvarme, retur</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_STATUS</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_TRACING_SPEC</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_INSUL_SPEC</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_PAINT_SPEC</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_MISC1</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_MISC2</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_MISC3</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_MISC4</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_MISC5</t>
+  </si>
+  <si>
+    <t>MAIN AREA</t>
+  </si>
+  <si>
+    <t>80 mm Mineral Wool</t>
+  </si>
+  <si>
+    <t>110 mm Mineral Wool</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>PN25</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>110°C</t>
+  </si>
+  <si>
+    <t>40°C</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_SPEC</t>
+  </si>
+  <si>
+    <t>30/03/2016</t>
   </si>
 </sst>
 </file>
@@ -603,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -622,6 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -907,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,15 +976,16 @@
     <col min="1" max="1" width="68.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="41" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="20.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="18" width="20.7109375" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -937,56 +996,104 @@
         <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -996,17 +1103,26 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1016,17 +1132,26 @@
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1036,17 +1161,26 @@
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1056,17 +1190,26 @@
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1076,17 +1219,26 @@
       <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1096,9 +1248,6 @@
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1106,10 +1255,22 @@
         <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1119,9 +1280,6 @@
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1129,10 +1287,22 @@
         <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1142,17 +1312,26 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -1162,17 +1341,26 @@
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1182,17 +1370,26 @@
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1202,17 +1399,26 @@
       <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1222,17 +1428,26 @@
       <c r="C15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1242,17 +1457,26 @@
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1262,17 +1486,26 @@
       <c r="C17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>125</v>
       </c>
@@ -1282,17 +1515,26 @@
       <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1302,17 +1544,26 @@
       <c r="C19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
@@ -1322,17 +1573,26 @@
       <c r="C20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1342,17 +1602,26 @@
       <c r="C21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>56</v>
       </c>
@@ -1362,17 +1631,26 @@
       <c r="C22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>59</v>
       </c>
@@ -1382,17 +1660,26 @@
       <c r="C23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -1402,17 +1689,26 @@
       <c r="C24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>66</v>
       </c>
@@ -1422,17 +1718,26 @@
       <c r="C25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>68</v>
       </c>
@@ -1442,20 +1747,29 @@
       <c r="C26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -1465,20 +1779,29 @@
       <c r="C27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>72</v>
       </c>
@@ -1488,20 +1811,29 @@
       <c r="C28" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>74</v>
       </c>
@@ -1511,20 +1843,29 @@
       <c r="C29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="G29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>78</v>
       </c>
@@ -1534,20 +1875,29 @@
       <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
@@ -1557,17 +1907,26 @@
       <c r="C31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>82</v>
       </c>
@@ -1577,17 +1936,17 @@
       <c r="C32" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="G32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>83</v>
       </c>
@@ -1597,17 +1956,17 @@
       <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="G33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -1617,17 +1976,17 @@
       <c r="C34" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="G34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -1637,17 +1996,17 @@
       <c r="C35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="G35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>86</v>
       </c>
@@ -1657,17 +2016,17 @@
       <c r="C36" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="G36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
@@ -1677,17 +2036,17 @@
       <c r="C37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="G37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>88</v>
       </c>
@@ -1697,17 +2056,17 @@
       <c r="C38" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>93</v>
       </c>
@@ -1717,17 +2076,17 @@
       <c r="C39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -1737,17 +2096,17 @@
       <c r="C40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="G40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>99</v>
       </c>
@@ -1757,20 +2116,20 @@
       <c r="C41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="G41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>127</v>
       </c>
@@ -1780,20 +2139,20 @@
       <c r="C42" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="G42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>103</v>
       </c>
@@ -1803,17 +2162,17 @@
       <c r="C43" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="F43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="G43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>106</v>
       </c>
@@ -1823,13 +2182,13 @@
       <c r="C44" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="I44" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1843,9 +2202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1853,79 +2210,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>160</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>161</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2578,7 +3002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Work with supports cont.
</commit_message>
<xml_diff>
--- a/PCF-exporter/PCF_DEVELOPEMENT_01.xlsx
+++ b/PCF-exporter/PCF_DEVELOPEMENT_01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\PCF-exporter\PCF-exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pcf-exporter\PCF-exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="COMP" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="204">
   <si>
     <t>ELBW</t>
   </si>
@@ -611,12 +611,81 @@
   </si>
   <si>
     <t>30/03/2016</t>
+  </si>
+  <si>
+    <t>Support Symbolic: ANC</t>
+  </si>
+  <si>
+    <t>SUPPORT</t>
+  </si>
+  <si>
+    <t>ANCH</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
+    <t>ASSY_SH_CL</t>
+  </si>
+  <si>
+    <t>Support Symbolic: B+</t>
+  </si>
+  <si>
+    <t>SKID</t>
+  </si>
+  <si>
+    <t>Pipe support</t>
+  </si>
+  <si>
+    <t>ASSY_LE_DL</t>
+  </si>
+  <si>
+    <t>Support Symbolic: CAN</t>
+  </si>
+  <si>
+    <t>SPRG</t>
+  </si>
+  <si>
+    <t>Can spring support</t>
+  </si>
+  <si>
+    <t>ASSY_RR_SR_DH</t>
+  </si>
+  <si>
+    <t>Support Symbolic: GUI</t>
+  </si>
+  <si>
+    <t>GUID</t>
+  </si>
+  <si>
+    <t>Guide support</t>
+  </si>
+  <si>
+    <t>ASSY_RR_SR_CL</t>
+  </si>
+  <si>
+    <t>Support Symbolic: GUI + B+</t>
+  </si>
+  <si>
+    <t>ASSY_VS_SR_DB</t>
+  </si>
+  <si>
+    <t>Support Symbolic: HGR</t>
+  </si>
+  <si>
+    <t>HANG</t>
+  </si>
+  <si>
+    <t>Hanger spring support</t>
+  </si>
+  <si>
+    <t>PCF_ELEM_SUPPORT_NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -778,6 +847,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -813,6 +899,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -965,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S45" sqref="S45:S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,10 +1085,11 @@
     <col min="8" max="8" width="20.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="41" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="18" width="20.7109375" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="19" max="19" width="21.42578125" style="3" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1040,8 +1144,11 @@
       <c r="R1" s="13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
@@ -1067,7 +1174,7 @@
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
@@ -1093,7 +1200,7 @@
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1122,7 +1229,7 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1151,7 +1258,7 @@
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1287,7 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -1209,7 +1316,7 @@
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1238,7 +1345,7 @@
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1270,7 +1377,7 @@
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1302,7 +1409,7 @@
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -1331,7 +1438,7 @@
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -1360,7 +1467,7 @@
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1389,7 +1496,7 @@
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1418,7 +1525,7 @@
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -1447,7 +1554,7 @@
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1946,7 +2053,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>83</v>
       </c>
@@ -1966,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -1986,7 +2093,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -2006,7 +2113,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>86</v>
       </c>
@@ -2026,7 +2133,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
@@ -2046,7 +2153,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>88</v>
       </c>
@@ -2066,7 +2173,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>93</v>
       </c>
@@ -2086,7 +2193,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -2106,7 +2213,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>99</v>
       </c>
@@ -2129,7 +2236,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>127</v>
       </c>
@@ -2152,7 +2259,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>103</v>
       </c>
@@ -2172,7 +2279,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>106</v>
       </c>
@@ -2190,6 +2297,126 @@
       </c>
       <c r="I44" s="3" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="S45" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="S46" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="S47" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="S48" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="S49" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="S50" s="12" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2202,7 +2429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>